<commit_message>
Latest data: for Scottish Mon Feb  1 18:04:15 UTC 2021
</commit_message>
<xml_diff>
--- a/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B1%2BFebruary%2B2021.xlsx
+++ b/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B1%2BFebruary%2B2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u208525\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u208525\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uG1127\A29207215\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -246,7 +246,7 @@
 </t>
   </si>
   <si>
-    <t>Please note that no data has been received from the NHS Tayside laboratory since Saturday 30th January</t>
+    <t>Please note that no data has been received from the NHS Tayside laboratory since Saturday 30th January though positive cases for Tayside will continue to rise as other labs continue to report these tests.</t>
   </si>
 </sst>
 </file>
@@ -7681,10 +7681,10 @@
   <dimension ref="A1:S346"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B308" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B317" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A336" sqref="A336"/>
+      <selection pane="bottomRight" activeCell="R335" sqref="R335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -71699,7 +71699,7 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -71724,7 +71724,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2021-02-01T11:14:38Z</value>
+      <value order="0">2021-02-01T17:50:12Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -71739,13 +71739,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA46394867</value>
+      <value order="0">vA46412980</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">69.131</value>
+      <value order="0">69.132</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">592</value>
+      <value order="0">593</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -71785,7 +71785,7 @@
 </metadata>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>